<commit_message>
committing the new asset details test class
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/AssetNameTestData.xlsx
+++ b/src/test/resources/TestData/AssetNameTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ruchika.Behura\git\VRT\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2155C27E-AE7D-4236-BED3-303D3B797698}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD225B11-574C-4601-A57B-9B5C64A458D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="847" firstSheet="32" activeTab="40" xr2:uid="{88CC17F3-0530-4FB5-9C07-02E67965A03F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="847" firstSheet="32" activeTab="39" xr2:uid="{88CC17F3-0530-4FB5-9C07-02E67965A03F}"/>
   </bookViews>
   <sheets>
     <sheet name="ASST02" sheetId="2" r:id="rId1"/>
@@ -1954,7 +1954,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4752" uniqueCount="1271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4746" uniqueCount="1270">
   <si>
     <t>Name</t>
   </si>
@@ -5707,9 +5707,6 @@
   </si>
   <si>
     <t>BB4</t>
-  </si>
-  <si>
-    <t>CC5</t>
   </si>
   <si>
     <t>45A</t>
@@ -20073,10 +20070,10 @@
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F885FD-1FF7-4875-B905-EA1FDA89DE03}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20111,54 +20108,6 @@
       </c>
       <c r="B4" s="18">
         <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>1248</v>
-      </c>
-      <c r="B5" s="18">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>1249</v>
-      </c>
-      <c r="B6" s="18">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>1250</v>
-      </c>
-      <c r="B7" s="18">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>1251</v>
-      </c>
-      <c r="B8" s="18">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>1252</v>
-      </c>
-      <c r="B9" s="18">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
-        <v>1253</v>
-      </c>
-      <c r="B10" s="13">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -20189,7 +20138,7 @@
         <v>1245</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -20197,7 +20146,7 @@
         <v>1246</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -20213,7 +20162,7 @@
         <v>1248</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -20229,12 +20178,12 @@
         <v>1250</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>1236</v>
@@ -20242,18 +20191,18 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B10" s="18" t="s">
         <v>1259</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>1260</v>
       </c>
     </row>
   </sheetData>
@@ -20997,8 +20946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90B4D6E5-D0B5-4085-AA8C-2F4DB91423EA}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21008,36 +20957,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>1261</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="5" t="s">
         <v>1262</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>1263</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="25" t="s">
         <v>1264</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>1265</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>1266</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" t="s">
         <v>1267</v>
-      </c>
-      <c r="E2" t="s">
-        <v>1268</v>
       </c>
     </row>
   </sheetData>
@@ -21049,7 +20998,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDEEAC7D-06A4-4075-B7D2-CBB6553C7070}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -21060,12 +21009,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>